<commit_message>
Charter revision added out of scope
</commit_message>
<xml_diff>
--- a/sampledata.xlsx
+++ b/sampledata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531367\Desktop\fall 2018\gdp\gdp pro\project-charter-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{50C42E65-27FF-49A1-A3F3-5C2986EDEE16}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8E69F85E-7611-4265-844F-D2C44E36D074}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{1EFB7A57-4E6A-4ACE-AE29-9C18350302D9}"/>
   </bookViews>
@@ -226,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -238,7 +238,6 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -557,7 +556,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +863,7 @@
       <c r="J13" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made necessary changes to the index file as per Dr. Case review
</commit_message>
<xml_diff>
--- a/sampledata.xlsx
+++ b/sampledata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531499\Desktop\GDP1\project-charter-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531373\GDP\project-charter-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A8D15D-1DB1-4DD3-B14D-E7FE50201974}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C76D683-9D66-4255-9AD5-B9939C7AC4FB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{1EFB7A57-4E6A-4ACE-AE29-9C18350302D9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Event_ID</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>stadium4</t>
-  </si>
-  <si>
-    <t>10/15/20186:00 PM</t>
   </si>
   <si>
     <t>james</t>
@@ -165,7 +162,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -203,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -239,15 +236,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -256,13 +297,56 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{117AFC82-C2E9-4F74-9ECE-904337A7DE77}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -573,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D6C220-6919-4D46-9C0E-5584257DD180}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,410 +672,433 @@
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="K1" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+      <c r="I1" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <v>1000</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>43342</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>3</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="3">
         <v>100</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <v>1000</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="4">
         <v>43342</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="5">
         <v>0.78125</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>1001</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>43353</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <v>101</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <v>1000</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="4">
         <v>43343</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="5">
         <v>0.80208333333333337</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>1002</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>43384</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>0.625</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>4</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="I5" s="5">
+      <c r="G5" s="1"/>
+      <c r="I5" s="3">
         <v>102</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <v>1001</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="4">
         <v>43353</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="5">
         <v>0.6875</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>1003</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>43388</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>0.75</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>4</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>103</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <v>1003</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4">
+        <v>43388</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="I8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>100</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1234567890</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3">
+        <v>10</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="3">
+        <v>63.7</v>
+      </c>
+      <c r="L10" s="3">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>101</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6">
+        <v>7890123456</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="3">
+        <v>11</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="3">
+        <v>74.7</v>
+      </c>
+      <c r="L11" s="3">
+        <v>89.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>102</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1987654321</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="3">
+        <v>12</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="3">
+        <v>83.8</v>
+      </c>
+      <c r="L12" s="3">
+        <v>84.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>103</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C13" s="6">
+        <v>6605280000</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="3">
+        <v>13</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="3">
+        <v>89.5</v>
+      </c>
+      <c r="L13" s="3">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>11</v>
       </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="3">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>12</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>13</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>100</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="8">
-        <v>1234567890</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="5">
-        <v>10</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="5">
-        <v>63.7</v>
-      </c>
-      <c r="J10" s="5">
-        <v>78.900000000000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>101</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="8">
-        <v>7890123456</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="5">
-        <v>11</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="5">
-        <v>74.7</v>
-      </c>
-      <c r="J11" s="5">
-        <v>89.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>102</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="8">
-        <v>1987654321</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="5">
-        <v>12</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="5">
-        <v>83.8</v>
-      </c>
-      <c r="J12" s="5">
-        <v>84.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>103</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="8">
-        <v>6605280000</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="5">
-        <v>13</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="5">
-        <v>89.5</v>
-      </c>
-      <c r="J13" s="5">
-        <v>88.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>10</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="5">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>11</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="5">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>12</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="5">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>13</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="D20" s="3">
         <v>888</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="I8:L8"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" xr:uid="{D9580F1F-D089-4226-9C90-A8AEF94EE369}"/>
     <hyperlink ref="D11" r:id="rId2" xr:uid="{3ED2BF57-EC66-4112-881C-6B8C79D1717C}"/>
@@ -999,5 +1106,6 @@
     <hyperlink ref="D13" r:id="rId4" xr:uid="{B9EF14D6-4471-4A74-A1A1-810FF90E266D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>